<commit_message>
One final test run and cleanup of the repo
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -14,15 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$19</definedName>
-  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="14">
   <si>
     <t>ActualSize</t>
   </si>
@@ -39,9 +36,6 @@
     <t>ExpectedSize</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -54,9 +48,6 @@
     <t>True</t>
   </si>
   <si>
-    <t>http://f586e1a7.bwtest-aws.pravala.com/384MB.jar</t>
-  </si>
-  <si>
     <t>Success</t>
   </si>
   <si>
@@ -66,17 +57,17 @@
     <t>./data/testResult.jar</t>
   </si>
   <si>
-    <t>Manually Added Notes</t>
-  </si>
-  <si>
-    <t>Total File Size is 384MB which is smaller than the total amount of data we tried to download from the server. The amount downloaded equals the total file size. This failure should be expected</t>
+    <t>Manual Notes</t>
+  </si>
+  <si>
+    <t>Ive confirmed that the data we downloaded matches what is available on the server. Because we were requesting chunks that went beyond the size of the data on the server we should have expected this failure.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,13 +82,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,28 +127,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,22 +445,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="56.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="82.109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,19 +485,16 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -527,23 +505,19 @@
       <c r="E2">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1048576</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -554,23 +528,19 @@
       <c r="E3">
         <v>1048576</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
+      <c r="F3" t="s">
+        <v>9</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16777216</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -581,23 +551,19 @@
       <c r="E4">
         <v>16777216</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
+      <c r="F4" t="s">
+        <v>9</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -608,23 +574,19 @@
       <c r="E5">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
+      <c r="F5" t="s">
+        <v>9</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4194304</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -635,23 +597,19 @@
       <c r="E6">
         <v>4194304</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
+      <c r="F6" t="s">
+        <v>9</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>67108864</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -662,23 +620,19 @@
       <c r="E7">
         <v>67108864</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
+      <c r="F7" t="s">
+        <v>9</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>40</v>
@@ -689,23 +643,19 @@
       <c r="E8">
         <v>160</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>10</v>
+      <c r="F8" t="s">
+        <v>9</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>41943040</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>40</v>
@@ -716,23 +666,19 @@
       <c r="E9">
         <v>41943040</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
+      <c r="F9" t="s">
+        <v>9</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
       </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>402654087</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -743,25 +689,22 @@
       <c r="E10">
         <v>671088640</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -772,23 +715,19 @@
       <c r="E11">
         <v>4</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>10</v>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1048576</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -799,23 +738,19 @@
       <c r="E12">
         <v>1048576</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>10</v>
+      <c r="F12" t="s">
+        <v>9</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>16777216</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -826,23 +761,19 @@
       <c r="E13">
         <v>16777216</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>10</v>
+      <c r="F13" t="s">
+        <v>9</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -853,23 +784,19 @@
       <c r="E14">
         <v>16</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>10</v>
+      <c r="F14" t="s">
+        <v>9</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
       </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4194304</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -880,23 +807,19 @@
       <c r="E15">
         <v>4194304</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
+      <c r="F15" t="s">
+        <v>9</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
       </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>67108864</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -907,23 +830,19 @@
       <c r="E16">
         <v>67108864</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>10</v>
+      <c r="F16" t="s">
+        <v>9</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
       </c>
-      <c r="H16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>40</v>
@@ -934,23 +853,19 @@
       <c r="E17">
         <v>160</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>10</v>
+      <c r="F17" t="s">
+        <v>9</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
       </c>
-      <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>41943040</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>40</v>
@@ -961,23 +876,19 @@
       <c r="E18">
         <v>41943040</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>10</v>
+      <c r="F18" t="s">
+        <v>9</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
       </c>
-      <c r="H18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>402654087</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19">
         <v>40</v>
@@ -988,40 +899,17 @@
       <c r="E19">
         <v>671088640</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" t="s">
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>15</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="F13" r:id="rId12"/>
-    <hyperlink ref="F14" r:id="rId13"/>
-    <hyperlink ref="F15" r:id="rId14"/>
-    <hyperlink ref="F16" r:id="rId15"/>
-    <hyperlink ref="F17" r:id="rId16"/>
-    <hyperlink ref="F18" r:id="rId17"/>
-    <hyperlink ref="F19" r:id="rId18"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>